<commit_message>
Match 4 closeness centrality
</commit_message>
<xml_diff>
--- a/Fourth_Match/4.RM3-MAL2 Stat 19.8.18.xlsx
+++ b/Fourth_Match/4.RM3-MAL2 Stat 19.8.18.xlsx
@@ -331,18 +331,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="26" min="11" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="1" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="26" min="11" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="1" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1132,22 +1132,24 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1192,7 +1194,9 @@
       <c r="A2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="n">
+        <v>0.175175786616693</v>
+      </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="F2" s="8"/>
@@ -1207,7 +1211,9 @@
       <c r="A3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="8" t="n">
+        <v>0.589435431269796</v>
+      </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>

</xml_diff>